<commit_message>
feat: Add Selenium Only domains and improve logging/progress display
Implemented enhancements for the hybrid image fetching script (requests with Selenium fallback):

Key changes:
- Added `SELENIUM_ONLY_DOMAINS` list to process specific unstable domains (eBay, Mercari) directly with Selenium, speeding up their processing.
- Introduced `--debug` option to enable detailed debug logging (including step timings) to a file (`scraping_debug.log`).
- Suppressed verbose internal logs from `urllib3` and `selenium` libraries.
- Improved progress display to show `X/Y items` based on the actual count of URLs to process.
- Added display of cumulative elapsed time after each URL processing and total script execution time at the end.
- Reduced Selenium fallback wait time (`time.sleep`) to 1 second.
- Removed unnecessary comments and HTML debug code.
- Enhanced error logging with traceback information and improved code formatting.
</commit_message>
<xml_diff>
--- a/画像取得.xlsx
+++ b/画像取得.xlsx
@@ -464,6 +464,31 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>10</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="952500" cy="952500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="10" name="Image 10" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -946,14 +971,22 @@
       </c>
       <c r="D10" s="12" t="n"/>
     </row>
-    <row r="11" ht="58.5" customHeight="1">
+    <row r="11" ht="77" customHeight="1">
       <c r="A11" s="3">
         <f>ROW()-1</f>
         <v/>
       </c>
-      <c r="B11" s="8" t="n"/>
-      <c r="C11" s="8" t="n"/>
-      <c r="D11" s="9" t="n"/>
+      <c r="B11" s="8" t="inlineStr">
+        <is>
+          <t>https://www.buyma.com/item/107182714/</t>
+        </is>
+      </c>
+      <c r="C11" s="8" t="inlineStr">
+        <is>
+          <t>https://cdn-images.buyma.com/imgdata/item/240531/0107182714/623187252/428.jpg</t>
+        </is>
+      </c>
+      <c r="D11" s="12" t="n"/>
     </row>
     <row r="12" ht="58.5" customHeight="1">
       <c r="A12" s="3">

</xml_diff>